<commit_message>
update Log4J + screenshot in report
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Java workspace\DataDrivenUdemy\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{72BDE977-BB79-48F1-A030-CA56EE451E10}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="108" windowWidth="14352" windowHeight="4692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,11 +22,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Tai</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>Giang</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Abcd20</t>
+  </si>
+  <si>
+    <t>Test1000</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,6 +101,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -109,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +185,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -177,6 +237,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -352,38 +429,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>